<commit_message>
Fixed some oversights with the new banners. Added outfits to a significant ammount of NPCs.
</commit_message>
<xml_diff>
--- a/Items+Troops Spreadsheets/HYW Regular Troops.xlsx
+++ b/Items+Troops Spreadsheets/HYW Regular Troops.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoanne\Desktop\HYW Repo\Items+Troops Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB6DBA0-54EE-4883-A96A-81C670A1D065}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6FCFB16-3DED-4C62-83AB-EDB5705CF1B8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{DC5A1941-EC3F-4B6C-990E-24E904CBA2AB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="3" activeTab="5" xr2:uid="{DC5A1941-EC3F-4B6C-990E-24E904CBA2AB}"/>
   </bookViews>
   <sheets>
     <sheet name="France" sheetId="1" r:id="rId1"/>
     <sheet name="England" sheetId="2" r:id="rId2"/>
     <sheet name="Burgundy" sheetId="3" r:id="rId3"/>
     <sheet name="Bretagne" sheetId="4" r:id="rId4"/>
+    <sheet name="Item sets for nobles" sheetId="5" r:id="rId5"/>
+    <sheet name="Item sets for commoners" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="119">
   <si>
     <t>Name Sing.</t>
   </si>
@@ -280,6 +282,111 @@
   </si>
   <si>
     <t>Crossbows</t>
+  </si>
+  <si>
+    <t>itm_h_bascinet_great,itm_heraldic_churburg_13_brass_tabard,itm_b_shynbaulds,itm_g_hourglass_gauntlets</t>
+  </si>
+  <si>
+    <t>itm_h_bascinet_oniontop,itm_heraldic_tunic_new,itm_g_finger_gauntlets,itm_b_steel_greaves_full</t>
+  </si>
+  <si>
+    <t>itm_h_klappvisier_pigface_open,itm_heraldic_churburg_13_tabard,itm_b_shynbaulds,itm_g_plate_mittens</t>
+  </si>
+  <si>
+    <t>itm_h_zitta_bascinet_novisor,itm_heraldic_early_transitional,itm_b_splinted_greaves_spurs,itm_g_wisby_gauntlets_black</t>
+  </si>
+  <si>
+    <t>itm_h_zitta_bascinet,itm_heraldic_churburg_13_brass_tabard,itm_b_shynbaulds,itm_g_hourglass_gauntlets_ornate</t>
+  </si>
+  <si>
+    <t>itm_h_klappvisier_pigface,itm_mail_long_surcoat_new_heraldic,itm_b_steel_greaves,itm_g_mail_gauntlets</t>
+  </si>
+  <si>
+    <t>itm_h_zitta_bascinet,itm_brigandine_b_heraldic,itm_b_shynbaulds,itm_g_demi_gauntlets</t>
+  </si>
+  <si>
+    <t>itm_h_zitta_bascinet_novisor,itm_heraldic_mail_tabard,itm_b_leather_boots,itm_g_mail_gauntlets</t>
+  </si>
+  <si>
+    <t>itm_h_klappvisier_pigface,itm_heraldic_early_transitional,itm_b_steel_greaves,itm_g_demi_gauntlets</t>
+  </si>
+  <si>
+    <t>itm_h_houndskull_thick,itm_heraldic_plate,itm_b_shynbaulds,itm_g_plate_mittens</t>
+  </si>
+  <si>
+    <t>itm_h_bascinet_great,itm_heraldic_tunic_new,itm_b_steel_greaves,itm_g_demi_gauntlets</t>
+  </si>
+  <si>
+    <t>itm_h_zitta_bascinet,itm_mail_long_surcoat_new_heraldic,itm_b_mail_boots,itm_g_mail_gauntlets</t>
+  </si>
+  <si>
+    <t>itm_h_hounskull_narf,itm_brigandine_b_heraldic,itm_b_shynbaulds,itm_g_hourglass_gauntlets</t>
+  </si>
+  <si>
+    <t>Tavern Keepers</t>
+  </si>
+  <si>
+    <t>itm_a_tavern_keeper_shirt,itm_b_hosen_poulaines_custom</t>
+  </si>
+  <si>
+    <t>itm_a_commoner_apron,itm_b_hosen_shoes_custom</t>
+  </si>
+  <si>
+    <t>itm_a_peasant_coat,itm_b_ankle_boots</t>
+  </si>
+  <si>
+    <t>itm_a_peasant_shirt_white,itm_b_hosen_poulaines_custom</t>
+  </si>
+  <si>
+    <t>itm_h_felt_hat_b_black,itm_a_commoner_apron,itm_b_hosen_shoes_custom</t>
+  </si>
+  <si>
+    <t>itm_h_highlander_beret_brown,itm_a_tavern_keeper_shirt,itm_b_hosen_poulaines_custom</t>
+  </si>
+  <si>
+    <t>itm_h_highlander_beret_white,itm_a_peasant_shirt_white,itm_b_hosen_poulaines_custom</t>
+  </si>
+  <si>
+    <t>itm_a_peasant_man_custom,itm_b_hosen_poulaines_custom</t>
+  </si>
+  <si>
+    <t>itm_h_felt_hat_b_brown,itm_a_peasant_man_custom,itm_b_hosen_poulaines_custom</t>
+  </si>
+  <si>
+    <t>Misc.</t>
+  </si>
+  <si>
+    <t>itm_h_felt_hat_b_white,itm_a_peasant_coat,itm_b_hosen_poulaines_custom</t>
+  </si>
+  <si>
+    <t>itm_a_tabard,itm_b_hosen_poulaines_custom</t>
+  </si>
+  <si>
+    <t>itm_h_highlander_beret_brown,itm_a_noble_shirt_brown,itm_b_hosen_poulaines_custom</t>
+  </si>
+  <si>
+    <t>itm_h_highlander_beret_red,itm_a_noble_shirt_red,itm_b_hosen_poulaines_custom</t>
+  </si>
+  <si>
+    <t>itm_h_highlander_beret_white,itm_a_noble_shirt_white,itm_b_hosen_poulaines_custom</t>
+  </si>
+  <si>
+    <t>itm_h_highlander_beret_black,itm_a_noble_shirt_black,itm_b_hosen_poulaines_custom</t>
+  </si>
+  <si>
+    <t>itm_h_highlander_beret_green,itm_a_noble_shirt_green,itm_b_hosen_poulaines_custom</t>
+  </si>
+  <si>
+    <t>itm_h_highlander_beret_blue,itm_a_noble_shirt_blue,itm_b_hosen_poulaines_custom</t>
+  </si>
+  <si>
+    <t>itm_a_commoner_apron,itm_b_leather_boots</t>
+  </si>
+  <si>
+    <t>itm_a_leather_jerkin,itm_b_leather_boots</t>
+  </si>
+  <si>
+    <t>itm_a_merchant_outfit,itm_b_hosen_shoes_custom</t>
   </si>
 </sst>
 </file>
@@ -773,7 +880,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D610EC-41D7-4EF8-B146-7C083064CBFC}">
   <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="B3" sqref="B3"/>
     </sheetView>
@@ -4640,4 +4747,230 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B3880EF-030F-4ABD-B34F-02C0D6F40826}">
+  <dimension ref="A1:A13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="109.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ECD29B1-E571-41E3-B51F-203AD74D87B3}">
+  <dimension ref="A1:A26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="82.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- Updated Noble troops stats. - Added Equipment to SangLys Mercenary
</commit_message>
<xml_diff>
--- a/Items+Troops Spreadsheets/HYW Regular Troops.xlsx
+++ b/Items+Troops Spreadsheets/HYW Regular Troops.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoanne\Desktop\HYW Repo\Items+Troops Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6FCFB16-3DED-4C62-83AB-EDB5705CF1B8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD55D89C-8506-4988-95F2-D771A0E93DA8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="3" activeTab="5" xr2:uid="{DC5A1941-EC3F-4B6C-990E-24E904CBA2AB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="6" activeTab="9" xr2:uid="{DC5A1941-EC3F-4B6C-990E-24E904CBA2AB}"/>
   </bookViews>
   <sheets>
     <sheet name="France" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,10 @@
     <sheet name="Bretagne" sheetId="4" r:id="rId4"/>
     <sheet name="Item sets for nobles" sheetId="5" r:id="rId5"/>
     <sheet name="Item sets for commoners" sheetId="6" r:id="rId6"/>
+    <sheet name="French Nobles" sheetId="7" r:id="rId7"/>
+    <sheet name="English Nobles" sheetId="8" r:id="rId8"/>
+    <sheet name="Burgundian Nobles" sheetId="9" r:id="rId9"/>
+    <sheet name="Breton Nobles" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -30,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="154">
   <si>
     <t>Name Sing.</t>
   </si>
@@ -387,6 +391,111 @@
   </si>
   <si>
     <t>itm_a_merchant_outfit,itm_b_hosen_shoes_custom</t>
+  </si>
+  <si>
+    <t>Captain</t>
+  </si>
+  <si>
+    <t>Captains</t>
+  </si>
+  <si>
+    <t>Bachelier</t>
+  </si>
+  <si>
+    <t>Bacheliers</t>
+  </si>
+  <si>
+    <t>Banneret</t>
+  </si>
+  <si>
+    <t>Bannerets</t>
+  </si>
+  <si>
+    <t>Lancier</t>
+  </si>
+  <si>
+    <t>Lanciers</t>
+  </si>
+  <si>
+    <t>Écuyer</t>
+  </si>
+  <si>
+    <t>Écuyers</t>
+  </si>
+  <si>
+    <t>Knight</t>
+  </si>
+  <si>
+    <t>Heavy Knight</t>
+  </si>
+  <si>
+    <t>Saint Georges Knight</t>
+  </si>
+  <si>
+    <t>Saint Georges Knights</t>
+  </si>
+  <si>
+    <t>Squire</t>
+  </si>
+  <si>
+    <t>Squires</t>
+  </si>
+  <si>
+    <t>Three Lions Guard</t>
+  </si>
+  <si>
+    <t>Knights</t>
+  </si>
+  <si>
+    <t>Three Lions Guards</t>
+  </si>
+  <si>
+    <t>Longbowman Captain</t>
+  </si>
+  <si>
+    <t>Longbowmen Captains</t>
+  </si>
+  <si>
+    <t>Heavy Knights</t>
+  </si>
+  <si>
+    <t>Guard</t>
+  </si>
+  <si>
+    <t>Elite Guard</t>
+  </si>
+  <si>
+    <t>Elite Guards</t>
+  </si>
+  <si>
+    <t>Iron Knight</t>
+  </si>
+  <si>
+    <t>Crossbowman Captain</t>
+  </si>
+  <si>
+    <t>Crossbowmen Captains</t>
+  </si>
+  <si>
+    <t>Noble</t>
+  </si>
+  <si>
+    <t>Nobles</t>
+  </si>
+  <si>
+    <t>Noble Swordsman</t>
+  </si>
+  <si>
+    <t>Noble Swordsmen</t>
+  </si>
+  <si>
+    <t>Honour Guard</t>
+  </si>
+  <si>
+    <t>Ermine Knight</t>
+  </si>
+  <si>
+    <t>Ermine Knights</t>
   </si>
 </sst>
 </file>
@@ -408,7 +517,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -454,6 +563,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -533,7 +648,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -562,6 +677,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -881,8 +1002,8 @@
   <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B3" sqref="B3"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1904,13 +2025,617 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09205900-6A83-4A0B-BA08-01057134C9D5}">
+  <dimension ref="A1:J20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P14" sqref="P14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10">
+        <v>25</v>
+      </c>
+      <c r="C3" s="10">
+        <v>28</v>
+      </c>
+      <c r="D3" s="10">
+        <v>32</v>
+      </c>
+      <c r="E3" s="10">
+        <v>32</v>
+      </c>
+      <c r="G3" s="12">
+        <v>25</v>
+      </c>
+      <c r="H3" s="12">
+        <v>28</v>
+      </c>
+      <c r="I3" s="12">
+        <v>30</v>
+      </c>
+      <c r="J3" s="12">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10">
+        <v>20</v>
+      </c>
+      <c r="C4" s="10">
+        <v>22</v>
+      </c>
+      <c r="D4" s="10">
+        <v>25</v>
+      </c>
+      <c r="E4" s="10">
+        <v>26</v>
+      </c>
+      <c r="G4" s="12">
+        <v>20</v>
+      </c>
+      <c r="H4" s="12">
+        <v>22</v>
+      </c>
+      <c r="I4" s="12">
+        <v>24</v>
+      </c>
+      <c r="J4" s="12">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10">
+        <v>20</v>
+      </c>
+      <c r="C5" s="10">
+        <v>22</v>
+      </c>
+      <c r="D5" s="10">
+        <v>25</v>
+      </c>
+      <c r="E5" s="10">
+        <v>24</v>
+      </c>
+      <c r="G5" s="12">
+        <v>20</v>
+      </c>
+      <c r="H5" s="12">
+        <v>22</v>
+      </c>
+      <c r="I5" s="12">
+        <v>24</v>
+      </c>
+      <c r="J5" s="12">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10">
+        <v>5</v>
+      </c>
+      <c r="C6" s="10">
+        <v>6</v>
+      </c>
+      <c r="D6" s="10">
+        <v>8</v>
+      </c>
+      <c r="E6" s="10">
+        <v>7</v>
+      </c>
+      <c r="G6" s="12">
+        <v>5</v>
+      </c>
+      <c r="H6" s="12">
+        <v>6</v>
+      </c>
+      <c r="I6" s="12">
+        <v>7</v>
+      </c>
+      <c r="J6" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10">
+        <v>5</v>
+      </c>
+      <c r="C7" s="10">
+        <v>5</v>
+      </c>
+      <c r="D7" s="10">
+        <v>7</v>
+      </c>
+      <c r="E7" s="10">
+        <v>8</v>
+      </c>
+      <c r="G7" s="12">
+        <v>5</v>
+      </c>
+      <c r="H7" s="12">
+        <v>5</v>
+      </c>
+      <c r="I7" s="12">
+        <v>6</v>
+      </c>
+      <c r="J7" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10">
+        <v>0</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0</v>
+      </c>
+      <c r="E8" s="10">
+        <v>0</v>
+      </c>
+      <c r="G8" s="12">
+        <v>0</v>
+      </c>
+      <c r="H8" s="12">
+        <v>0</v>
+      </c>
+      <c r="I8" s="12">
+        <v>0</v>
+      </c>
+      <c r="J8" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="10">
+        <v>0</v>
+      </c>
+      <c r="C9" s="10">
+        <v>0</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0</v>
+      </c>
+      <c r="E9" s="10">
+        <v>0</v>
+      </c>
+      <c r="G9" s="12">
+        <v>0</v>
+      </c>
+      <c r="H9" s="12">
+        <v>0</v>
+      </c>
+      <c r="I9" s="12">
+        <v>0</v>
+      </c>
+      <c r="J9" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="10">
+        <v>0</v>
+      </c>
+      <c r="C10" s="10">
+        <v>3</v>
+      </c>
+      <c r="D10" s="10">
+        <v>0</v>
+      </c>
+      <c r="E10" s="10">
+        <v>0</v>
+      </c>
+      <c r="G10" s="12">
+        <v>3</v>
+      </c>
+      <c r="H10" s="12">
+        <v>3</v>
+      </c>
+      <c r="I10" s="12">
+        <v>4</v>
+      </c>
+      <c r="J10" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="10">
+        <v>4</v>
+      </c>
+      <c r="C11" s="10">
+        <v>4</v>
+      </c>
+      <c r="D11" s="10">
+        <v>5</v>
+      </c>
+      <c r="E11" s="10">
+        <v>5</v>
+      </c>
+      <c r="G11" s="12">
+        <v>4</v>
+      </c>
+      <c r="H11" s="12">
+        <v>4</v>
+      </c>
+      <c r="I11" s="12">
+        <v>4</v>
+      </c>
+      <c r="J11" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="10">
+        <v>5</v>
+      </c>
+      <c r="C12" s="10">
+        <v>5</v>
+      </c>
+      <c r="D12" s="10">
+        <v>7</v>
+      </c>
+      <c r="E12" s="10">
+        <v>6</v>
+      </c>
+      <c r="G12" s="12">
+        <v>5</v>
+      </c>
+      <c r="H12" s="12">
+        <v>5</v>
+      </c>
+      <c r="I12" s="12">
+        <v>6</v>
+      </c>
+      <c r="J12" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="10">
+        <v>0</v>
+      </c>
+      <c r="C13" s="10">
+        <v>0</v>
+      </c>
+      <c r="D13" s="10">
+        <v>0</v>
+      </c>
+      <c r="E13" s="10">
+        <v>0</v>
+      </c>
+      <c r="G13" s="12">
+        <v>3</v>
+      </c>
+      <c r="H13" s="12">
+        <v>4</v>
+      </c>
+      <c r="I13" s="12">
+        <v>5</v>
+      </c>
+      <c r="J13" s="12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="10">
+        <v>0</v>
+      </c>
+      <c r="C14" s="10">
+        <v>0</v>
+      </c>
+      <c r="D14" s="10">
+        <v>0</v>
+      </c>
+      <c r="E14" s="10">
+        <v>0</v>
+      </c>
+      <c r="G14" s="12">
+        <v>0</v>
+      </c>
+      <c r="H14" s="12">
+        <v>0</v>
+      </c>
+      <c r="I14" s="12">
+        <v>0</v>
+      </c>
+      <c r="J14" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="10">
+        <v>160</v>
+      </c>
+      <c r="C15" s="10">
+        <v>180</v>
+      </c>
+      <c r="D15" s="10">
+        <v>250</v>
+      </c>
+      <c r="E15" s="10">
+        <v>100</v>
+      </c>
+      <c r="G15" s="12">
+        <v>150</v>
+      </c>
+      <c r="H15" s="12">
+        <v>180</v>
+      </c>
+      <c r="I15" s="12">
+        <v>200</v>
+      </c>
+      <c r="J15" s="12">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="10">
+        <v>160</v>
+      </c>
+      <c r="C16" s="10">
+        <v>180</v>
+      </c>
+      <c r="D16" s="10">
+        <v>280</v>
+      </c>
+      <c r="E16" s="10">
+        <v>100</v>
+      </c>
+      <c r="G16" s="12">
+        <v>150</v>
+      </c>
+      <c r="H16" s="12">
+        <v>180</v>
+      </c>
+      <c r="I16" s="12">
+        <v>200</v>
+      </c>
+      <c r="J16" s="12">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="10">
+        <v>160</v>
+      </c>
+      <c r="C17" s="10">
+        <v>180</v>
+      </c>
+      <c r="D17" s="10">
+        <v>100</v>
+      </c>
+      <c r="E17" s="10">
+        <v>280</v>
+      </c>
+      <c r="G17" s="12">
+        <v>150</v>
+      </c>
+      <c r="H17" s="12">
+        <v>180</v>
+      </c>
+      <c r="I17" s="12">
+        <v>200</v>
+      </c>
+      <c r="J17" s="12">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="10">
+        <v>100</v>
+      </c>
+      <c r="C18" s="10">
+        <v>100</v>
+      </c>
+      <c r="D18" s="10">
+        <v>100</v>
+      </c>
+      <c r="E18" s="10">
+        <v>100</v>
+      </c>
+      <c r="G18" s="12">
+        <v>100</v>
+      </c>
+      <c r="H18" s="12">
+        <v>100</v>
+      </c>
+      <c r="I18" s="12">
+        <v>100</v>
+      </c>
+      <c r="J18" s="12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="10">
+        <v>100</v>
+      </c>
+      <c r="C19" s="10">
+        <v>100</v>
+      </c>
+      <c r="D19" s="10">
+        <v>100</v>
+      </c>
+      <c r="E19" s="10">
+        <v>100</v>
+      </c>
+      <c r="G19" s="12">
+        <v>100</v>
+      </c>
+      <c r="H19" s="12">
+        <v>100</v>
+      </c>
+      <c r="I19" s="12">
+        <v>100</v>
+      </c>
+      <c r="J19" s="12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="10">
+        <v>100</v>
+      </c>
+      <c r="C20" s="10">
+        <v>100</v>
+      </c>
+      <c r="D20" s="10">
+        <v>100</v>
+      </c>
+      <c r="E20" s="10">
+        <v>100</v>
+      </c>
+      <c r="G20" s="12">
+        <v>100</v>
+      </c>
+      <c r="H20" s="12">
+        <v>100</v>
+      </c>
+      <c r="I20" s="12">
+        <v>100</v>
+      </c>
+      <c r="J20" s="12">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C48F968-6098-45C2-90F4-E48BCC11AF74}">
   <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A19" sqref="A19"/>
+      <selection pane="topRight" activeCell="O3" sqref="O3:O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3969,7 +4694,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A19" sqref="A19"/>
+      <selection pane="topRight" sqref="A1:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4836,7 +5561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5ECD29B1-E571-41E3-B51F-203AD74D87B3}">
   <dimension ref="A1:A26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
@@ -4973,4 +5698,1813 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D487E40-5146-4C6B-93D8-C3C5513BACDF}">
+  <dimension ref="A1:J20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" customWidth="1"/>
+    <col min="9" max="9" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10">
+        <v>25</v>
+      </c>
+      <c r="C3" s="10">
+        <v>28</v>
+      </c>
+      <c r="D3" s="10">
+        <v>30</v>
+      </c>
+      <c r="E3" s="10">
+        <v>35</v>
+      </c>
+      <c r="G3" s="12">
+        <v>25</v>
+      </c>
+      <c r="H3" s="12">
+        <v>28</v>
+      </c>
+      <c r="I3" s="12">
+        <v>30</v>
+      </c>
+      <c r="J3" s="12">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10">
+        <v>20</v>
+      </c>
+      <c r="C4" s="10">
+        <v>22</v>
+      </c>
+      <c r="D4" s="10">
+        <v>24</v>
+      </c>
+      <c r="E4" s="10">
+        <v>28</v>
+      </c>
+      <c r="G4" s="12">
+        <v>20</v>
+      </c>
+      <c r="H4" s="12">
+        <v>22</v>
+      </c>
+      <c r="I4" s="12">
+        <v>24</v>
+      </c>
+      <c r="J4" s="12">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10">
+        <v>20</v>
+      </c>
+      <c r="C5" s="10">
+        <v>22</v>
+      </c>
+      <c r="D5" s="10">
+        <v>24</v>
+      </c>
+      <c r="E5" s="10">
+        <v>28</v>
+      </c>
+      <c r="G5" s="12">
+        <v>20</v>
+      </c>
+      <c r="H5" s="12">
+        <v>22</v>
+      </c>
+      <c r="I5" s="12">
+        <v>24</v>
+      </c>
+      <c r="J5" s="12">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10">
+        <v>5</v>
+      </c>
+      <c r="C6" s="10">
+        <v>6</v>
+      </c>
+      <c r="D6" s="10">
+        <v>7</v>
+      </c>
+      <c r="E6" s="10">
+        <v>8</v>
+      </c>
+      <c r="G6" s="12">
+        <v>6</v>
+      </c>
+      <c r="H6" s="12">
+        <v>7</v>
+      </c>
+      <c r="I6" s="12">
+        <v>8</v>
+      </c>
+      <c r="J6" s="12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10">
+        <v>5</v>
+      </c>
+      <c r="C7" s="10">
+        <v>5</v>
+      </c>
+      <c r="D7" s="10">
+        <v>6</v>
+      </c>
+      <c r="E7" s="10">
+        <v>8</v>
+      </c>
+      <c r="G7" s="12">
+        <v>5</v>
+      </c>
+      <c r="H7" s="12">
+        <v>5</v>
+      </c>
+      <c r="I7" s="12">
+        <v>6</v>
+      </c>
+      <c r="J7" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10">
+        <v>0</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0</v>
+      </c>
+      <c r="E8" s="10">
+        <v>0</v>
+      </c>
+      <c r="G8" s="12">
+        <v>0</v>
+      </c>
+      <c r="H8" s="12">
+        <v>0</v>
+      </c>
+      <c r="I8" s="12">
+        <v>0</v>
+      </c>
+      <c r="J8" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="10">
+        <v>0</v>
+      </c>
+      <c r="C9" s="10">
+        <v>0</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0</v>
+      </c>
+      <c r="E9" s="10">
+        <v>0</v>
+      </c>
+      <c r="G9" s="12">
+        <v>0</v>
+      </c>
+      <c r="H9" s="12">
+        <v>0</v>
+      </c>
+      <c r="I9" s="12">
+        <v>0</v>
+      </c>
+      <c r="J9" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="10">
+        <v>3</v>
+      </c>
+      <c r="C10" s="10">
+        <v>3</v>
+      </c>
+      <c r="D10" s="10">
+        <v>4</v>
+      </c>
+      <c r="E10" s="10">
+        <v>4</v>
+      </c>
+      <c r="G10" s="12">
+        <v>3</v>
+      </c>
+      <c r="H10" s="12">
+        <v>3</v>
+      </c>
+      <c r="I10" s="12">
+        <v>4</v>
+      </c>
+      <c r="J10" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="10">
+        <v>4</v>
+      </c>
+      <c r="C11" s="10">
+        <v>4</v>
+      </c>
+      <c r="D11" s="10">
+        <v>4</v>
+      </c>
+      <c r="E11" s="10">
+        <v>4</v>
+      </c>
+      <c r="G11" s="12">
+        <v>4</v>
+      </c>
+      <c r="H11" s="12">
+        <v>4</v>
+      </c>
+      <c r="I11" s="12">
+        <v>4</v>
+      </c>
+      <c r="J11" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="10">
+        <v>5</v>
+      </c>
+      <c r="C12" s="10">
+        <v>5</v>
+      </c>
+      <c r="D12" s="10">
+        <v>6</v>
+      </c>
+      <c r="E12" s="10">
+        <v>8</v>
+      </c>
+      <c r="G12" s="12">
+        <v>5</v>
+      </c>
+      <c r="H12" s="12">
+        <v>5</v>
+      </c>
+      <c r="I12" s="12">
+        <v>6</v>
+      </c>
+      <c r="J12" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="10">
+        <v>0</v>
+      </c>
+      <c r="C13" s="10">
+        <v>0</v>
+      </c>
+      <c r="D13" s="10">
+        <v>0</v>
+      </c>
+      <c r="E13" s="10">
+        <v>0</v>
+      </c>
+      <c r="G13" s="12">
+        <v>4</v>
+      </c>
+      <c r="H13" s="12">
+        <v>5</v>
+      </c>
+      <c r="I13" s="12">
+        <v>6</v>
+      </c>
+      <c r="J13" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="10">
+        <v>0</v>
+      </c>
+      <c r="C14" s="10">
+        <v>0</v>
+      </c>
+      <c r="D14" s="10">
+        <v>0</v>
+      </c>
+      <c r="E14" s="10">
+        <v>0</v>
+      </c>
+      <c r="G14" s="12">
+        <v>0</v>
+      </c>
+      <c r="H14" s="12">
+        <v>0</v>
+      </c>
+      <c r="I14" s="12">
+        <v>0</v>
+      </c>
+      <c r="J14" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="10">
+        <v>160</v>
+      </c>
+      <c r="C15" s="10">
+        <v>180</v>
+      </c>
+      <c r="D15" s="10">
+        <v>200</v>
+      </c>
+      <c r="E15" s="10">
+        <v>250</v>
+      </c>
+      <c r="G15" s="12">
+        <v>180</v>
+      </c>
+      <c r="H15" s="12">
+        <v>200</v>
+      </c>
+      <c r="I15" s="12">
+        <v>220</v>
+      </c>
+      <c r="J15" s="12">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="10">
+        <v>160</v>
+      </c>
+      <c r="C16" s="10">
+        <v>180</v>
+      </c>
+      <c r="D16" s="10">
+        <v>200</v>
+      </c>
+      <c r="E16" s="10">
+        <v>250</v>
+      </c>
+      <c r="G16" s="12">
+        <v>180</v>
+      </c>
+      <c r="H16" s="12">
+        <v>200</v>
+      </c>
+      <c r="I16" s="12">
+        <v>220</v>
+      </c>
+      <c r="J16" s="12">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="10">
+        <v>160</v>
+      </c>
+      <c r="C17" s="10">
+        <v>180</v>
+      </c>
+      <c r="D17" s="10">
+        <v>200</v>
+      </c>
+      <c r="E17" s="10">
+        <v>250</v>
+      </c>
+      <c r="G17" s="12">
+        <v>180</v>
+      </c>
+      <c r="H17" s="12">
+        <v>200</v>
+      </c>
+      <c r="I17" s="12">
+        <v>220</v>
+      </c>
+      <c r="J17" s="12">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="10">
+        <v>100</v>
+      </c>
+      <c r="C18" s="10">
+        <v>100</v>
+      </c>
+      <c r="D18" s="10">
+        <v>100</v>
+      </c>
+      <c r="E18" s="10">
+        <v>100</v>
+      </c>
+      <c r="G18" s="12">
+        <v>100</v>
+      </c>
+      <c r="H18" s="12">
+        <v>100</v>
+      </c>
+      <c r="I18" s="12">
+        <v>100</v>
+      </c>
+      <c r="J18" s="12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="10">
+        <v>100</v>
+      </c>
+      <c r="C19" s="10">
+        <v>100</v>
+      </c>
+      <c r="D19" s="10">
+        <v>100</v>
+      </c>
+      <c r="E19" s="10">
+        <v>100</v>
+      </c>
+      <c r="G19" s="12">
+        <v>100</v>
+      </c>
+      <c r="H19" s="12">
+        <v>100</v>
+      </c>
+      <c r="I19" s="12">
+        <v>100</v>
+      </c>
+      <c r="J19" s="12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="10">
+        <v>100</v>
+      </c>
+      <c r="C20" s="10">
+        <v>100</v>
+      </c>
+      <c r="D20" s="10">
+        <v>100</v>
+      </c>
+      <c r="E20" s="10">
+        <v>100</v>
+      </c>
+      <c r="G20" s="12">
+        <v>100</v>
+      </c>
+      <c r="H20" s="12">
+        <v>100</v>
+      </c>
+      <c r="I20" s="12">
+        <v>100</v>
+      </c>
+      <c r="J20" s="12">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BDB3DC1-432C-4354-96F1-8DB95BAB3F3A}">
+  <dimension ref="A1:J20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" sqref="A1:A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10">
+        <v>25</v>
+      </c>
+      <c r="C3" s="10">
+        <v>30</v>
+      </c>
+      <c r="D3" s="10">
+        <v>35</v>
+      </c>
+      <c r="E3" s="8">
+        <v>28</v>
+      </c>
+      <c r="G3" s="12">
+        <v>25</v>
+      </c>
+      <c r="H3" s="12">
+        <v>28</v>
+      </c>
+      <c r="I3" s="12">
+        <v>30</v>
+      </c>
+      <c r="J3" s="12">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10">
+        <v>20</v>
+      </c>
+      <c r="C4" s="10">
+        <v>24</v>
+      </c>
+      <c r="D4" s="10">
+        <v>28</v>
+      </c>
+      <c r="E4" s="8">
+        <v>20</v>
+      </c>
+      <c r="G4" s="12">
+        <v>20</v>
+      </c>
+      <c r="H4" s="12">
+        <v>22</v>
+      </c>
+      <c r="I4" s="12">
+        <v>24</v>
+      </c>
+      <c r="J4" s="12">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10">
+        <v>20</v>
+      </c>
+      <c r="C5" s="10">
+        <v>24</v>
+      </c>
+      <c r="D5" s="10">
+        <v>28</v>
+      </c>
+      <c r="E5" s="8">
+        <v>20</v>
+      </c>
+      <c r="G5" s="12">
+        <v>20</v>
+      </c>
+      <c r="H5" s="12">
+        <v>22</v>
+      </c>
+      <c r="I5" s="12">
+        <v>24</v>
+      </c>
+      <c r="J5" s="12">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10">
+        <v>5</v>
+      </c>
+      <c r="C6" s="10">
+        <v>7</v>
+      </c>
+      <c r="D6" s="10">
+        <v>8</v>
+      </c>
+      <c r="E6" s="8">
+        <v>5</v>
+      </c>
+      <c r="G6" s="12">
+        <v>5</v>
+      </c>
+      <c r="H6" s="12">
+        <v>6</v>
+      </c>
+      <c r="I6" s="12">
+        <v>7</v>
+      </c>
+      <c r="J6" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10">
+        <v>5</v>
+      </c>
+      <c r="C7" s="10">
+        <v>7</v>
+      </c>
+      <c r="D7" s="10">
+        <v>8</v>
+      </c>
+      <c r="E7" s="8">
+        <v>5</v>
+      </c>
+      <c r="G7" s="12">
+        <v>5</v>
+      </c>
+      <c r="H7" s="12">
+        <v>5</v>
+      </c>
+      <c r="I7" s="12">
+        <v>6</v>
+      </c>
+      <c r="J7" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10">
+        <v>0</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="12">
+        <v>0</v>
+      </c>
+      <c r="H8" s="12">
+        <v>0</v>
+      </c>
+      <c r="I8" s="12">
+        <v>0</v>
+      </c>
+      <c r="J8" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="10">
+        <v>0</v>
+      </c>
+      <c r="C9" s="10">
+        <v>0</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0</v>
+      </c>
+      <c r="E9" s="8">
+        <v>6</v>
+      </c>
+      <c r="G9" s="12">
+        <v>0</v>
+      </c>
+      <c r="H9" s="12">
+        <v>0</v>
+      </c>
+      <c r="I9" s="12">
+        <v>0</v>
+      </c>
+      <c r="J9" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="10">
+        <v>3</v>
+      </c>
+      <c r="C10" s="10">
+        <v>4</v>
+      </c>
+      <c r="D10" s="10">
+        <v>5</v>
+      </c>
+      <c r="E10" s="8">
+        <v>2</v>
+      </c>
+      <c r="G10" s="12">
+        <v>3</v>
+      </c>
+      <c r="H10" s="12">
+        <v>3</v>
+      </c>
+      <c r="I10" s="12">
+        <v>4</v>
+      </c>
+      <c r="J10" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="10">
+        <v>4</v>
+      </c>
+      <c r="C11" s="10">
+        <v>4</v>
+      </c>
+      <c r="D11" s="10">
+        <v>4</v>
+      </c>
+      <c r="E11" s="8">
+        <v>4</v>
+      </c>
+      <c r="G11" s="12">
+        <v>4</v>
+      </c>
+      <c r="H11" s="12">
+        <v>4</v>
+      </c>
+      <c r="I11" s="12">
+        <v>4</v>
+      </c>
+      <c r="J11" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="10">
+        <v>5</v>
+      </c>
+      <c r="C12" s="10">
+        <v>6</v>
+      </c>
+      <c r="D12" s="10">
+        <v>8</v>
+      </c>
+      <c r="E12" s="8">
+        <v>5</v>
+      </c>
+      <c r="G12" s="12">
+        <v>5</v>
+      </c>
+      <c r="H12" s="12">
+        <v>5</v>
+      </c>
+      <c r="I12" s="12">
+        <v>6</v>
+      </c>
+      <c r="J12" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="10">
+        <v>0</v>
+      </c>
+      <c r="C13" s="10">
+        <v>0</v>
+      </c>
+      <c r="D13" s="10">
+        <v>0</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0</v>
+      </c>
+      <c r="G13" s="12">
+        <v>3</v>
+      </c>
+      <c r="H13" s="12">
+        <v>4</v>
+      </c>
+      <c r="I13" s="12">
+        <v>5</v>
+      </c>
+      <c r="J13" s="12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="10">
+        <v>0</v>
+      </c>
+      <c r="C14" s="10">
+        <v>0</v>
+      </c>
+      <c r="D14" s="10">
+        <v>0</v>
+      </c>
+      <c r="E14" s="8">
+        <v>0</v>
+      </c>
+      <c r="G14" s="12">
+        <v>0</v>
+      </c>
+      <c r="H14" s="12">
+        <v>0</v>
+      </c>
+      <c r="I14" s="12">
+        <v>0</v>
+      </c>
+      <c r="J14" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="10">
+        <v>180</v>
+      </c>
+      <c r="C15" s="10">
+        <v>220</v>
+      </c>
+      <c r="D15" s="10">
+        <v>260</v>
+      </c>
+      <c r="E15" s="8">
+        <v>180</v>
+      </c>
+      <c r="G15" s="12">
+        <v>150</v>
+      </c>
+      <c r="H15" s="12">
+        <v>180</v>
+      </c>
+      <c r="I15" s="12">
+        <v>200</v>
+      </c>
+      <c r="J15" s="12">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="10">
+        <v>180</v>
+      </c>
+      <c r="C16" s="10">
+        <v>220</v>
+      </c>
+      <c r="D16" s="10">
+        <v>260</v>
+      </c>
+      <c r="E16" s="8">
+        <v>180</v>
+      </c>
+      <c r="G16" s="12">
+        <v>150</v>
+      </c>
+      <c r="H16" s="12">
+        <v>180</v>
+      </c>
+      <c r="I16" s="12">
+        <v>200</v>
+      </c>
+      <c r="J16" s="12">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="10">
+        <v>180</v>
+      </c>
+      <c r="C17" s="10">
+        <v>220</v>
+      </c>
+      <c r="D17" s="10">
+        <v>260</v>
+      </c>
+      <c r="E17" s="8">
+        <v>100</v>
+      </c>
+      <c r="G17" s="12">
+        <v>150</v>
+      </c>
+      <c r="H17" s="12">
+        <v>180</v>
+      </c>
+      <c r="I17" s="12">
+        <v>200</v>
+      </c>
+      <c r="J17" s="12">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="10">
+        <v>100</v>
+      </c>
+      <c r="C18" s="10">
+        <v>100</v>
+      </c>
+      <c r="D18" s="10">
+        <v>100</v>
+      </c>
+      <c r="E18" s="8">
+        <v>220</v>
+      </c>
+      <c r="G18" s="12">
+        <v>100</v>
+      </c>
+      <c r="H18" s="12">
+        <v>100</v>
+      </c>
+      <c r="I18" s="12">
+        <v>100</v>
+      </c>
+      <c r="J18" s="12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="10">
+        <v>100</v>
+      </c>
+      <c r="C19" s="10">
+        <v>100</v>
+      </c>
+      <c r="D19" s="10">
+        <v>100</v>
+      </c>
+      <c r="E19" s="8">
+        <v>100</v>
+      </c>
+      <c r="G19" s="12">
+        <v>100</v>
+      </c>
+      <c r="H19" s="12">
+        <v>100</v>
+      </c>
+      <c r="I19" s="12">
+        <v>100</v>
+      </c>
+      <c r="J19" s="12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="10">
+        <v>100</v>
+      </c>
+      <c r="C20" s="10">
+        <v>100</v>
+      </c>
+      <c r="D20" s="10">
+        <v>100</v>
+      </c>
+      <c r="E20" s="8">
+        <v>100</v>
+      </c>
+      <c r="G20" s="12">
+        <v>100</v>
+      </c>
+      <c r="H20" s="12">
+        <v>100</v>
+      </c>
+      <c r="I20" s="12">
+        <v>100</v>
+      </c>
+      <c r="J20" s="12">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D628C025-DB4C-40D8-BAB4-876849ED9353}">
+  <dimension ref="A1:J20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10">
+        <v>25</v>
+      </c>
+      <c r="C3" s="10">
+        <v>28</v>
+      </c>
+      <c r="D3" s="10">
+        <v>30</v>
+      </c>
+      <c r="F3" s="12">
+        <v>25</v>
+      </c>
+      <c r="G3" s="12">
+        <v>28</v>
+      </c>
+      <c r="H3" s="12">
+        <v>30</v>
+      </c>
+      <c r="I3" s="12">
+        <v>35</v>
+      </c>
+      <c r="J3" s="13">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10">
+        <v>20</v>
+      </c>
+      <c r="C4" s="10">
+        <v>22</v>
+      </c>
+      <c r="D4" s="10">
+        <v>24</v>
+      </c>
+      <c r="F4" s="12">
+        <v>20</v>
+      </c>
+      <c r="G4" s="12">
+        <v>22</v>
+      </c>
+      <c r="H4" s="12">
+        <v>24</v>
+      </c>
+      <c r="I4" s="12">
+        <v>28</v>
+      </c>
+      <c r="J4" s="13">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10">
+        <v>20</v>
+      </c>
+      <c r="C5" s="10">
+        <v>22</v>
+      </c>
+      <c r="D5" s="10">
+        <v>24</v>
+      </c>
+      <c r="F5" s="12">
+        <v>20</v>
+      </c>
+      <c r="G5" s="12">
+        <v>22</v>
+      </c>
+      <c r="H5" s="12">
+        <v>24</v>
+      </c>
+      <c r="I5" s="12">
+        <v>28</v>
+      </c>
+      <c r="J5" s="13">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10">
+        <v>5</v>
+      </c>
+      <c r="C6" s="10">
+        <v>6</v>
+      </c>
+      <c r="D6" s="10">
+        <v>7</v>
+      </c>
+      <c r="F6" s="12">
+        <v>6</v>
+      </c>
+      <c r="G6" s="12">
+        <v>7</v>
+      </c>
+      <c r="H6" s="12">
+        <v>8</v>
+      </c>
+      <c r="I6" s="12">
+        <v>9</v>
+      </c>
+      <c r="J6" s="13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10">
+        <v>5</v>
+      </c>
+      <c r="C7" s="10">
+        <v>5</v>
+      </c>
+      <c r="D7" s="10">
+        <v>6</v>
+      </c>
+      <c r="F7" s="12">
+        <v>5</v>
+      </c>
+      <c r="G7" s="12">
+        <v>5</v>
+      </c>
+      <c r="H7" s="12">
+        <v>6</v>
+      </c>
+      <c r="I7" s="12">
+        <v>8</v>
+      </c>
+      <c r="J7" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10">
+        <v>0</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0</v>
+      </c>
+      <c r="F8" s="12">
+        <v>0</v>
+      </c>
+      <c r="G8" s="12">
+        <v>0</v>
+      </c>
+      <c r="H8" s="12">
+        <v>0</v>
+      </c>
+      <c r="I8" s="12">
+        <v>0</v>
+      </c>
+      <c r="J8" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="10">
+        <v>0</v>
+      </c>
+      <c r="C9" s="10">
+        <v>0</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0</v>
+      </c>
+      <c r="F9" s="12">
+        <v>0</v>
+      </c>
+      <c r="G9" s="12">
+        <v>0</v>
+      </c>
+      <c r="H9" s="12">
+        <v>0</v>
+      </c>
+      <c r="I9" s="12">
+        <v>0</v>
+      </c>
+      <c r="J9" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="10">
+        <v>0</v>
+      </c>
+      <c r="C10" s="10">
+        <v>3</v>
+      </c>
+      <c r="D10" s="10">
+        <v>4</v>
+      </c>
+      <c r="F10" s="12">
+        <v>3</v>
+      </c>
+      <c r="G10" s="12">
+        <v>3</v>
+      </c>
+      <c r="H10" s="12">
+        <v>4</v>
+      </c>
+      <c r="I10" s="12">
+        <v>4</v>
+      </c>
+      <c r="J10" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="10">
+        <v>4</v>
+      </c>
+      <c r="C11" s="10">
+        <v>4</v>
+      </c>
+      <c r="D11" s="10">
+        <v>4</v>
+      </c>
+      <c r="F11" s="12">
+        <v>4</v>
+      </c>
+      <c r="G11" s="12">
+        <v>4</v>
+      </c>
+      <c r="H11" s="12">
+        <v>4</v>
+      </c>
+      <c r="I11" s="12">
+        <v>4</v>
+      </c>
+      <c r="J11" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="10">
+        <v>5</v>
+      </c>
+      <c r="C12" s="10">
+        <v>5</v>
+      </c>
+      <c r="D12" s="10">
+        <v>6</v>
+      </c>
+      <c r="F12" s="12">
+        <v>5</v>
+      </c>
+      <c r="G12" s="12">
+        <v>5</v>
+      </c>
+      <c r="H12" s="12">
+        <v>6</v>
+      </c>
+      <c r="I12" s="12">
+        <v>8</v>
+      </c>
+      <c r="J12" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="10">
+        <v>0</v>
+      </c>
+      <c r="C13" s="10">
+        <v>0</v>
+      </c>
+      <c r="D13" s="10">
+        <v>0</v>
+      </c>
+      <c r="F13" s="12">
+        <v>3</v>
+      </c>
+      <c r="G13" s="12">
+        <v>4</v>
+      </c>
+      <c r="H13" s="12">
+        <v>5</v>
+      </c>
+      <c r="I13" s="12">
+        <v>6</v>
+      </c>
+      <c r="J13" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="10">
+        <v>0</v>
+      </c>
+      <c r="C14" s="10">
+        <v>0</v>
+      </c>
+      <c r="D14" s="10">
+        <v>0</v>
+      </c>
+      <c r="F14" s="12">
+        <v>0</v>
+      </c>
+      <c r="G14" s="12">
+        <v>0</v>
+      </c>
+      <c r="H14" s="12">
+        <v>0</v>
+      </c>
+      <c r="I14" s="12">
+        <v>0</v>
+      </c>
+      <c r="J14" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="10">
+        <v>160</v>
+      </c>
+      <c r="C15" s="10">
+        <v>180</v>
+      </c>
+      <c r="D15" s="10">
+        <v>200</v>
+      </c>
+      <c r="F15" s="12">
+        <v>170</v>
+      </c>
+      <c r="G15" s="12">
+        <v>190</v>
+      </c>
+      <c r="H15" s="12">
+        <v>215</v>
+      </c>
+      <c r="I15" s="12">
+        <v>250</v>
+      </c>
+      <c r="J15" s="13">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="10">
+        <v>160</v>
+      </c>
+      <c r="C16" s="10">
+        <v>180</v>
+      </c>
+      <c r="D16" s="10">
+        <v>200</v>
+      </c>
+      <c r="F16" s="12">
+        <v>170</v>
+      </c>
+      <c r="G16" s="12">
+        <v>190</v>
+      </c>
+      <c r="H16" s="12">
+        <v>215</v>
+      </c>
+      <c r="I16" s="12">
+        <v>250</v>
+      </c>
+      <c r="J16" s="13">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="10">
+        <v>160</v>
+      </c>
+      <c r="C17" s="10">
+        <v>180</v>
+      </c>
+      <c r="D17" s="10">
+        <v>200</v>
+      </c>
+      <c r="F17" s="12">
+        <v>170</v>
+      </c>
+      <c r="G17" s="12">
+        <v>190</v>
+      </c>
+      <c r="H17" s="12">
+        <v>215</v>
+      </c>
+      <c r="I17" s="12">
+        <v>250</v>
+      </c>
+      <c r="J17" s="13">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="10">
+        <v>100</v>
+      </c>
+      <c r="C18" s="10">
+        <v>100</v>
+      </c>
+      <c r="D18" s="10">
+        <v>100</v>
+      </c>
+      <c r="F18" s="12">
+        <v>100</v>
+      </c>
+      <c r="G18" s="12">
+        <v>100</v>
+      </c>
+      <c r="H18" s="12">
+        <v>100</v>
+      </c>
+      <c r="I18" s="12">
+        <v>100</v>
+      </c>
+      <c r="J18" s="13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="10">
+        <v>100</v>
+      </c>
+      <c r="C19" s="10">
+        <v>100</v>
+      </c>
+      <c r="D19" s="10">
+        <v>100</v>
+      </c>
+      <c r="F19" s="12">
+        <v>100</v>
+      </c>
+      <c r="G19" s="12">
+        <v>100</v>
+      </c>
+      <c r="H19" s="12">
+        <v>100</v>
+      </c>
+      <c r="I19" s="12">
+        <v>100</v>
+      </c>
+      <c r="J19" s="13">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="10">
+        <v>100</v>
+      </c>
+      <c r="C20" s="10">
+        <v>100</v>
+      </c>
+      <c r="D20" s="10">
+        <v>100</v>
+      </c>
+      <c r="F20" s="12">
+        <v>100</v>
+      </c>
+      <c r="G20" s="12">
+        <v>100</v>
+      </c>
+      <c r="H20" s="12">
+        <v>100</v>
+      </c>
+      <c r="I20" s="12">
+        <v>100</v>
+      </c>
+      <c r="J20" s="13">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
- Updated stats of mercenary troops, rebels and iron skulls - Updated troop tree presentation to display the troops aforementioned.
</commit_message>
<xml_diff>
--- a/Items+Troops Spreadsheets/HYW Regular Troops.xlsx
+++ b/Items+Troops Spreadsheets/HYW Regular Troops.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yoanne\Desktop\HYW Repo\Items+Troops Spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD55D89C-8506-4988-95F2-D771A0E93DA8}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{720A7A96-DCE2-4E91-B262-E78F460218DE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="6" activeTab="9" xr2:uid="{DC5A1941-EC3F-4B6C-990E-24E904CBA2AB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="5" activeTab="11" xr2:uid="{DC5A1941-EC3F-4B6C-990E-24E904CBA2AB}"/>
   </bookViews>
   <sheets>
     <sheet name="France" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,8 @@
     <sheet name="English Nobles" sheetId="8" r:id="rId8"/>
     <sheet name="Burgundian Nobles" sheetId="9" r:id="rId9"/>
     <sheet name="Breton Nobles" sheetId="10" r:id="rId10"/>
+    <sheet name="Flemish Mercenaries" sheetId="11" r:id="rId11"/>
+    <sheet name="Generic Mercenaries" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="180">
   <si>
     <t>Name Sing.</t>
   </si>
@@ -496,6 +498,84 @@
   </si>
   <si>
     <t>Ermine Knights</t>
+  </si>
+  <si>
+    <t>Militia Crossbowmen</t>
+  </si>
+  <si>
+    <t>Heavy Crossbowman</t>
+  </si>
+  <si>
+    <t>Heavy Crossbowmen</t>
+  </si>
+  <si>
+    <t>German Knight</t>
+  </si>
+  <si>
+    <t>German Knights</t>
+  </si>
+  <si>
+    <t>Dismounted German Knight</t>
+  </si>
+  <si>
+    <t>Dismounted German Knights</t>
+  </si>
+  <si>
+    <t>Scout</t>
+  </si>
+  <si>
+    <t>Scouts</t>
+  </si>
+  <si>
+    <t>Light Cavalry</t>
+  </si>
+  <si>
+    <t>Light Cavalries</t>
+  </si>
+  <si>
+    <t>Cavalry</t>
+  </si>
+  <si>
+    <t>Watchman</t>
+  </si>
+  <si>
+    <t>Watchmen</t>
+  </si>
+  <si>
+    <t>Pavise Spearman</t>
+  </si>
+  <si>
+    <t>Pavise Spearmen</t>
+  </si>
+  <si>
+    <t>Caravan Guard</t>
+  </si>
+  <si>
+    <t>Caravan Guards</t>
+  </si>
+  <si>
+    <t>Swordsman</t>
+  </si>
+  <si>
+    <t>Swordsmen</t>
+  </si>
+  <si>
+    <t>Maceman</t>
+  </si>
+  <si>
+    <t>Macemen</t>
+  </si>
+  <si>
+    <t>Hired Blade</t>
+  </si>
+  <si>
+    <t>Hired Blades</t>
+  </si>
+  <si>
+    <t>Bowman</t>
+  </si>
+  <si>
+    <t>Bowmen</t>
   </si>
 </sst>
 </file>
@@ -1003,7 +1083,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H25" sqref="H25"/>
+      <selection pane="topRight" activeCell="N1" sqref="N1:P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2029,9 +2109,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09205900-6A83-4A0B-BA08-01057134C9D5}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="P14" sqref="P14"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" sqref="A1:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2629,13 +2709,1710 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AC5AE26-8066-473B-8C9E-09AC23968112}">
+  <dimension ref="A1:N20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" sqref="A1:A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" customWidth="1"/>
+    <col min="9" max="9" width="16" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" customWidth="1"/>
+    <col min="11" max="11" width="20" customWidth="1"/>
+    <col min="13" max="13" width="27.85546875" customWidth="1"/>
+    <col min="14" max="14" width="16.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="M2" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11">
+        <v>10</v>
+      </c>
+      <c r="C3" s="11">
+        <v>15</v>
+      </c>
+      <c r="D3" s="11">
+        <v>20</v>
+      </c>
+      <c r="E3" s="11">
+        <v>22</v>
+      </c>
+      <c r="G3" s="10">
+        <v>10</v>
+      </c>
+      <c r="H3" s="10">
+        <v>15</v>
+      </c>
+      <c r="I3" s="10">
+        <v>20</v>
+      </c>
+      <c r="J3" s="10">
+        <v>15</v>
+      </c>
+      <c r="K3" s="10">
+        <v>20</v>
+      </c>
+      <c r="M3" s="10">
+        <v>30</v>
+      </c>
+      <c r="N3" s="12">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="11">
+        <v>13</v>
+      </c>
+      <c r="C4" s="11">
+        <v>15</v>
+      </c>
+      <c r="D4" s="11">
+        <v>17</v>
+      </c>
+      <c r="E4" s="11">
+        <v>18</v>
+      </c>
+      <c r="G4" s="10">
+        <v>14</v>
+      </c>
+      <c r="H4" s="10">
+        <v>16</v>
+      </c>
+      <c r="I4" s="10">
+        <v>18</v>
+      </c>
+      <c r="J4" s="10">
+        <v>15</v>
+      </c>
+      <c r="K4" s="10">
+        <v>17</v>
+      </c>
+      <c r="M4" s="10">
+        <v>24</v>
+      </c>
+      <c r="N4" s="12">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11">
+        <v>12</v>
+      </c>
+      <c r="C5" s="11">
+        <v>13</v>
+      </c>
+      <c r="D5" s="11">
+        <v>15</v>
+      </c>
+      <c r="E5" s="11">
+        <v>16</v>
+      </c>
+      <c r="G5" s="10">
+        <v>10</v>
+      </c>
+      <c r="H5" s="10">
+        <v>12</v>
+      </c>
+      <c r="I5" s="10">
+        <v>15</v>
+      </c>
+      <c r="J5" s="10">
+        <v>13</v>
+      </c>
+      <c r="K5" s="10">
+        <v>16</v>
+      </c>
+      <c r="M5" s="10">
+        <v>24</v>
+      </c>
+      <c r="N5" s="12">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="11">
+        <v>2</v>
+      </c>
+      <c r="C6" s="11">
+        <v>3</v>
+      </c>
+      <c r="D6" s="11">
+        <v>4</v>
+      </c>
+      <c r="E6" s="11">
+        <v>4</v>
+      </c>
+      <c r="G6" s="10">
+        <v>3</v>
+      </c>
+      <c r="H6" s="10">
+        <v>4</v>
+      </c>
+      <c r="I6" s="10">
+        <v>5</v>
+      </c>
+      <c r="J6" s="10">
+        <v>3</v>
+      </c>
+      <c r="K6" s="10">
+        <v>4</v>
+      </c>
+      <c r="M6" s="10">
+        <v>7</v>
+      </c>
+      <c r="N6" s="12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="11">
+        <v>1</v>
+      </c>
+      <c r="C7" s="11">
+        <v>2</v>
+      </c>
+      <c r="D7" s="11">
+        <v>3</v>
+      </c>
+      <c r="E7" s="11">
+        <v>4</v>
+      </c>
+      <c r="G7" s="10">
+        <v>2</v>
+      </c>
+      <c r="H7" s="10">
+        <v>3</v>
+      </c>
+      <c r="I7" s="10">
+        <v>4</v>
+      </c>
+      <c r="J7" s="10">
+        <v>4</v>
+      </c>
+      <c r="K7" s="10">
+        <v>5</v>
+      </c>
+      <c r="M7" s="10">
+        <v>7</v>
+      </c>
+      <c r="N7" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="11">
+        <v>0</v>
+      </c>
+      <c r="C8" s="11">
+        <v>0</v>
+      </c>
+      <c r="D8" s="11">
+        <v>0</v>
+      </c>
+      <c r="E8" s="11">
+        <v>0</v>
+      </c>
+      <c r="G8" s="10">
+        <v>0</v>
+      </c>
+      <c r="H8" s="10">
+        <v>0</v>
+      </c>
+      <c r="I8" s="10">
+        <v>0</v>
+      </c>
+      <c r="J8" s="10">
+        <v>0</v>
+      </c>
+      <c r="K8" s="10">
+        <v>0</v>
+      </c>
+      <c r="M8" s="10">
+        <v>0</v>
+      </c>
+      <c r="N8" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="11">
+        <v>0</v>
+      </c>
+      <c r="C9" s="11">
+        <v>0</v>
+      </c>
+      <c r="D9" s="11">
+        <v>0</v>
+      </c>
+      <c r="E9" s="11">
+        <v>0</v>
+      </c>
+      <c r="G9" s="10">
+        <v>0</v>
+      </c>
+      <c r="H9" s="10">
+        <v>0</v>
+      </c>
+      <c r="I9" s="10">
+        <v>0</v>
+      </c>
+      <c r="J9" s="10">
+        <v>0</v>
+      </c>
+      <c r="K9" s="10">
+        <v>0</v>
+      </c>
+      <c r="M9" s="10">
+        <v>0</v>
+      </c>
+      <c r="N9" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="11">
+        <v>1</v>
+      </c>
+      <c r="C10" s="11">
+        <v>2</v>
+      </c>
+      <c r="D10" s="11">
+        <v>3</v>
+      </c>
+      <c r="E10" s="11">
+        <v>3</v>
+      </c>
+      <c r="G10" s="10">
+        <v>1</v>
+      </c>
+      <c r="H10" s="10">
+        <v>2</v>
+      </c>
+      <c r="I10" s="10">
+        <v>3</v>
+      </c>
+      <c r="J10" s="10">
+        <v>0</v>
+      </c>
+      <c r="K10" s="10">
+        <v>0</v>
+      </c>
+      <c r="M10" s="10">
+        <v>4</v>
+      </c>
+      <c r="N10" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="11">
+        <v>3</v>
+      </c>
+      <c r="C11" s="11">
+        <v>3</v>
+      </c>
+      <c r="D11" s="11">
+        <v>3</v>
+      </c>
+      <c r="E11" s="11">
+        <v>3</v>
+      </c>
+      <c r="G11" s="10">
+        <v>3</v>
+      </c>
+      <c r="H11" s="10">
+        <v>3</v>
+      </c>
+      <c r="I11" s="10">
+        <v>3</v>
+      </c>
+      <c r="J11" s="10">
+        <v>3</v>
+      </c>
+      <c r="K11" s="10">
+        <v>3</v>
+      </c>
+      <c r="M11" s="10">
+        <v>4</v>
+      </c>
+      <c r="N11" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="11">
+        <v>1</v>
+      </c>
+      <c r="C12" s="11">
+        <v>2</v>
+      </c>
+      <c r="D12" s="11">
+        <v>3</v>
+      </c>
+      <c r="E12" s="11">
+        <v>4</v>
+      </c>
+      <c r="G12" s="10">
+        <v>1</v>
+      </c>
+      <c r="H12" s="10">
+        <v>2</v>
+      </c>
+      <c r="I12" s="10">
+        <v>3</v>
+      </c>
+      <c r="J12" s="10">
+        <v>2</v>
+      </c>
+      <c r="K12" s="10">
+        <v>3</v>
+      </c>
+      <c r="M12" s="10">
+        <v>6</v>
+      </c>
+      <c r="N12" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="11">
+        <v>0</v>
+      </c>
+      <c r="C13" s="11">
+        <v>0</v>
+      </c>
+      <c r="D13" s="11">
+        <v>0</v>
+      </c>
+      <c r="E13" s="11">
+        <v>0</v>
+      </c>
+      <c r="G13" s="10">
+        <v>0</v>
+      </c>
+      <c r="H13" s="10">
+        <v>0</v>
+      </c>
+      <c r="I13" s="10">
+        <v>0</v>
+      </c>
+      <c r="J13" s="10">
+        <v>0</v>
+      </c>
+      <c r="K13" s="10">
+        <v>0</v>
+      </c>
+      <c r="M13" s="10">
+        <v>0</v>
+      </c>
+      <c r="N13" s="12">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="11">
+        <v>0</v>
+      </c>
+      <c r="C14" s="11">
+        <v>0</v>
+      </c>
+      <c r="D14" s="11">
+        <v>0</v>
+      </c>
+      <c r="E14" s="11">
+        <v>0</v>
+      </c>
+      <c r="G14" s="10">
+        <v>0</v>
+      </c>
+      <c r="H14" s="10">
+        <v>0</v>
+      </c>
+      <c r="I14" s="10">
+        <v>0</v>
+      </c>
+      <c r="J14" s="10">
+        <v>0</v>
+      </c>
+      <c r="K14" s="10">
+        <v>0</v>
+      </c>
+      <c r="M14" s="10">
+        <v>0</v>
+      </c>
+      <c r="N14" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="11">
+        <v>80</v>
+      </c>
+      <c r="C15" s="11">
+        <v>100</v>
+      </c>
+      <c r="D15" s="11">
+        <v>120</v>
+      </c>
+      <c r="E15" s="11">
+        <v>140</v>
+      </c>
+      <c r="G15" s="10">
+        <v>100</v>
+      </c>
+      <c r="H15" s="10">
+        <v>120</v>
+      </c>
+      <c r="I15" s="10">
+        <v>140</v>
+      </c>
+      <c r="J15" s="10">
+        <v>80</v>
+      </c>
+      <c r="K15" s="10">
+        <v>80</v>
+      </c>
+      <c r="M15" s="10">
+        <v>220</v>
+      </c>
+      <c r="N15" s="12">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="11">
+        <v>80</v>
+      </c>
+      <c r="C16" s="11">
+        <v>80</v>
+      </c>
+      <c r="D16" s="11">
+        <v>80</v>
+      </c>
+      <c r="E16" s="11">
+        <v>80</v>
+      </c>
+      <c r="G16" s="10">
+        <v>80</v>
+      </c>
+      <c r="H16" s="10">
+        <v>80</v>
+      </c>
+      <c r="I16" s="10">
+        <v>80</v>
+      </c>
+      <c r="J16" s="10">
+        <v>80</v>
+      </c>
+      <c r="K16" s="10">
+        <v>80</v>
+      </c>
+      <c r="M16" s="10">
+        <v>220</v>
+      </c>
+      <c r="N16" s="12">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="11">
+        <v>80</v>
+      </c>
+      <c r="C17" s="11">
+        <v>80</v>
+      </c>
+      <c r="D17" s="11">
+        <v>80</v>
+      </c>
+      <c r="E17" s="11">
+        <v>80</v>
+      </c>
+      <c r="G17" s="10">
+        <v>120</v>
+      </c>
+      <c r="H17" s="10">
+        <v>150</v>
+      </c>
+      <c r="I17" s="10">
+        <v>180</v>
+      </c>
+      <c r="J17" s="10">
+        <v>160</v>
+      </c>
+      <c r="K17" s="10">
+        <v>190</v>
+      </c>
+      <c r="M17" s="10">
+        <v>220</v>
+      </c>
+      <c r="N17" s="12">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="11">
+        <v>80</v>
+      </c>
+      <c r="C18" s="11">
+        <v>80</v>
+      </c>
+      <c r="D18" s="11">
+        <v>80</v>
+      </c>
+      <c r="E18" s="11">
+        <v>80</v>
+      </c>
+      <c r="G18" s="10">
+        <v>80</v>
+      </c>
+      <c r="H18" s="10">
+        <v>80</v>
+      </c>
+      <c r="I18" s="10">
+        <v>80</v>
+      </c>
+      <c r="J18" s="10">
+        <v>80</v>
+      </c>
+      <c r="K18" s="10">
+        <v>80</v>
+      </c>
+      <c r="M18" s="10">
+        <v>100</v>
+      </c>
+      <c r="N18" s="12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="11">
+        <v>120</v>
+      </c>
+      <c r="C19" s="11">
+        <v>140</v>
+      </c>
+      <c r="D19" s="11">
+        <v>160</v>
+      </c>
+      <c r="E19" s="11">
+        <v>180</v>
+      </c>
+      <c r="G19" s="10">
+        <v>80</v>
+      </c>
+      <c r="H19" s="10">
+        <v>80</v>
+      </c>
+      <c r="I19" s="10">
+        <v>80</v>
+      </c>
+      <c r="J19" s="10">
+        <v>80</v>
+      </c>
+      <c r="K19" s="10">
+        <v>80</v>
+      </c>
+      <c r="M19" s="10">
+        <v>100</v>
+      </c>
+      <c r="N19" s="12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="11">
+        <v>80</v>
+      </c>
+      <c r="C20" s="11">
+        <v>80</v>
+      </c>
+      <c r="D20" s="11">
+        <v>80</v>
+      </c>
+      <c r="E20" s="11">
+        <v>80</v>
+      </c>
+      <c r="G20" s="10">
+        <v>80</v>
+      </c>
+      <c r="H20" s="10">
+        <v>80</v>
+      </c>
+      <c r="I20" s="10">
+        <v>80</v>
+      </c>
+      <c r="J20" s="10">
+        <v>80</v>
+      </c>
+      <c r="K20" s="10">
+        <v>80</v>
+      </c>
+      <c r="M20" s="10">
+        <v>100</v>
+      </c>
+      <c r="N20" s="12">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CC88553-3C35-4B5A-9489-A454DD765A84}">
+  <dimension ref="A1:P20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N4" sqref="N4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" customWidth="1"/>
+    <col min="16" max="16" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="12">
+        <v>15</v>
+      </c>
+      <c r="C3" s="12">
+        <v>20</v>
+      </c>
+      <c r="D3" s="12">
+        <v>25</v>
+      </c>
+      <c r="F3" s="10">
+        <v>10</v>
+      </c>
+      <c r="G3" s="10">
+        <v>15</v>
+      </c>
+      <c r="H3" s="10">
+        <v>20</v>
+      </c>
+      <c r="I3" s="10">
+        <v>15</v>
+      </c>
+      <c r="J3" s="10">
+        <v>20</v>
+      </c>
+      <c r="K3" s="10">
+        <v>20</v>
+      </c>
+      <c r="L3" s="10">
+        <v>25</v>
+      </c>
+      <c r="N3" s="11">
+        <v>10</v>
+      </c>
+      <c r="O3" s="8">
+        <v>15</v>
+      </c>
+      <c r="P3" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="12">
+        <v>16</v>
+      </c>
+      <c r="C4" s="12">
+        <v>18</v>
+      </c>
+      <c r="D4" s="12">
+        <v>20</v>
+      </c>
+      <c r="F4" s="10">
+        <v>12</v>
+      </c>
+      <c r="G4" s="10">
+        <v>15</v>
+      </c>
+      <c r="H4" s="10">
+        <v>17</v>
+      </c>
+      <c r="I4" s="10">
+        <v>14</v>
+      </c>
+      <c r="J4" s="10">
+        <v>16</v>
+      </c>
+      <c r="K4" s="10">
+        <v>16</v>
+      </c>
+      <c r="L4" s="10">
+        <v>20</v>
+      </c>
+      <c r="N4" s="11">
+        <v>10</v>
+      </c>
+      <c r="O4" s="8">
+        <v>12</v>
+      </c>
+      <c r="P4" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12">
+        <v>16</v>
+      </c>
+      <c r="C5" s="12">
+        <v>18</v>
+      </c>
+      <c r="D5" s="12">
+        <v>20</v>
+      </c>
+      <c r="F5" s="10">
+        <v>12</v>
+      </c>
+      <c r="G5" s="10">
+        <v>13</v>
+      </c>
+      <c r="H5" s="10">
+        <v>15</v>
+      </c>
+      <c r="I5" s="10">
+        <v>14</v>
+      </c>
+      <c r="J5" s="10">
+        <v>16</v>
+      </c>
+      <c r="K5" s="10">
+        <v>16</v>
+      </c>
+      <c r="L5" s="10">
+        <v>20</v>
+      </c>
+      <c r="N5" s="11">
+        <v>12</v>
+      </c>
+      <c r="O5" s="8">
+        <v>14</v>
+      </c>
+      <c r="P5" s="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="12">
+        <v>3</v>
+      </c>
+      <c r="C6" s="12">
+        <v>4</v>
+      </c>
+      <c r="D6" s="12">
+        <v>5</v>
+      </c>
+      <c r="F6" s="10">
+        <v>2</v>
+      </c>
+      <c r="G6" s="10">
+        <v>4</v>
+      </c>
+      <c r="H6" s="10">
+        <v>5</v>
+      </c>
+      <c r="I6" s="10">
+        <v>3</v>
+      </c>
+      <c r="J6" s="10">
+        <v>4</v>
+      </c>
+      <c r="K6" s="10">
+        <v>4</v>
+      </c>
+      <c r="L6" s="10">
+        <v>5</v>
+      </c>
+      <c r="N6" s="11">
+        <v>1</v>
+      </c>
+      <c r="O6" s="8">
+        <v>2</v>
+      </c>
+      <c r="P6" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="12">
+        <v>3</v>
+      </c>
+      <c r="C7" s="12">
+        <v>4</v>
+      </c>
+      <c r="D7" s="12">
+        <v>5</v>
+      </c>
+      <c r="F7" s="10">
+        <v>2</v>
+      </c>
+      <c r="G7" s="10">
+        <v>2</v>
+      </c>
+      <c r="H7" s="10">
+        <v>3</v>
+      </c>
+      <c r="I7" s="10">
+        <v>3</v>
+      </c>
+      <c r="J7" s="10">
+        <v>4</v>
+      </c>
+      <c r="K7" s="10">
+        <v>4</v>
+      </c>
+      <c r="L7" s="10">
+        <v>5</v>
+      </c>
+      <c r="N7" s="11">
+        <v>1</v>
+      </c>
+      <c r="O7" s="8">
+        <v>2</v>
+      </c>
+      <c r="P7" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="12">
+        <v>0</v>
+      </c>
+      <c r="C8" s="12">
+        <v>0</v>
+      </c>
+      <c r="D8" s="12">
+        <v>0</v>
+      </c>
+      <c r="F8" s="10">
+        <v>0</v>
+      </c>
+      <c r="G8" s="10">
+        <v>0</v>
+      </c>
+      <c r="H8" s="10">
+        <v>0</v>
+      </c>
+      <c r="I8" s="10">
+        <v>0</v>
+      </c>
+      <c r="J8" s="10">
+        <v>0</v>
+      </c>
+      <c r="K8" s="10">
+        <v>0</v>
+      </c>
+      <c r="L8" s="10">
+        <v>0</v>
+      </c>
+      <c r="N8" s="11">
+        <v>0</v>
+      </c>
+      <c r="O8" s="8">
+        <v>0</v>
+      </c>
+      <c r="P8" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="12">
+        <v>0</v>
+      </c>
+      <c r="C9" s="12">
+        <v>0</v>
+      </c>
+      <c r="D9" s="12">
+        <v>0</v>
+      </c>
+      <c r="F9" s="10">
+        <v>0</v>
+      </c>
+      <c r="G9" s="10">
+        <v>0</v>
+      </c>
+      <c r="H9" s="10">
+        <v>0</v>
+      </c>
+      <c r="I9" s="10">
+        <v>0</v>
+      </c>
+      <c r="J9" s="10">
+        <v>0</v>
+      </c>
+      <c r="K9" s="10">
+        <v>0</v>
+      </c>
+      <c r="L9" s="10">
+        <v>0</v>
+      </c>
+      <c r="N9" s="11">
+        <v>2</v>
+      </c>
+      <c r="O9" s="8">
+        <v>3</v>
+      </c>
+      <c r="P9" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="12">
+        <v>1</v>
+      </c>
+      <c r="C10" s="12">
+        <v>2</v>
+      </c>
+      <c r="D10" s="12">
+        <v>3</v>
+      </c>
+      <c r="F10" s="10">
+        <v>1</v>
+      </c>
+      <c r="G10" s="10">
+        <v>2</v>
+      </c>
+      <c r="H10" s="10">
+        <v>3</v>
+      </c>
+      <c r="I10" s="10">
+        <v>2</v>
+      </c>
+      <c r="J10" s="10">
+        <v>3</v>
+      </c>
+      <c r="K10" s="10">
+        <v>3</v>
+      </c>
+      <c r="L10" s="10">
+        <v>0</v>
+      </c>
+      <c r="N10" s="11">
+        <v>0</v>
+      </c>
+      <c r="O10" s="8">
+        <v>0</v>
+      </c>
+      <c r="P10" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="12">
+        <v>3</v>
+      </c>
+      <c r="C11" s="12">
+        <v>4</v>
+      </c>
+      <c r="D11" s="12">
+        <v>4</v>
+      </c>
+      <c r="F11" s="10">
+        <v>3</v>
+      </c>
+      <c r="G11" s="10">
+        <v>3</v>
+      </c>
+      <c r="H11" s="10">
+        <v>3</v>
+      </c>
+      <c r="I11" s="10">
+        <v>3</v>
+      </c>
+      <c r="J11" s="10">
+        <v>3</v>
+      </c>
+      <c r="K11" s="10">
+        <v>3</v>
+      </c>
+      <c r="L11" s="10">
+        <v>4</v>
+      </c>
+      <c r="N11" s="11">
+        <v>4</v>
+      </c>
+      <c r="O11" s="8">
+        <v>4</v>
+      </c>
+      <c r="P11" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="12">
+        <v>3</v>
+      </c>
+      <c r="C12" s="12">
+        <v>4</v>
+      </c>
+      <c r="D12" s="12">
+        <v>5</v>
+      </c>
+      <c r="F12" s="10">
+        <v>1</v>
+      </c>
+      <c r="G12" s="10">
+        <v>1</v>
+      </c>
+      <c r="H12" s="10">
+        <v>2</v>
+      </c>
+      <c r="I12" s="10">
+        <v>1</v>
+      </c>
+      <c r="J12" s="10">
+        <v>2</v>
+      </c>
+      <c r="K12" s="10">
+        <v>2</v>
+      </c>
+      <c r="L12" s="10">
+        <v>5</v>
+      </c>
+      <c r="N12" s="11">
+        <v>1</v>
+      </c>
+      <c r="O12" s="8">
+        <v>2</v>
+      </c>
+      <c r="P12" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="12">
+        <v>2</v>
+      </c>
+      <c r="C13" s="12">
+        <v>3</v>
+      </c>
+      <c r="D13" s="12">
+        <v>4</v>
+      </c>
+      <c r="F13" s="10">
+        <v>0</v>
+      </c>
+      <c r="G13" s="10">
+        <v>0</v>
+      </c>
+      <c r="H13" s="10">
+        <v>0</v>
+      </c>
+      <c r="I13" s="10">
+        <v>0</v>
+      </c>
+      <c r="J13" s="10">
+        <v>0</v>
+      </c>
+      <c r="K13" s="10">
+        <v>0</v>
+      </c>
+      <c r="L13" s="10">
+        <v>0</v>
+      </c>
+      <c r="N13" s="11">
+        <v>0</v>
+      </c>
+      <c r="O13" s="8">
+        <v>0</v>
+      </c>
+      <c r="P13" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="25.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="12">
+        <v>0</v>
+      </c>
+      <c r="C14" s="12">
+        <v>0</v>
+      </c>
+      <c r="D14" s="12">
+        <v>0</v>
+      </c>
+      <c r="F14" s="10">
+        <v>0</v>
+      </c>
+      <c r="G14" s="10">
+        <v>0</v>
+      </c>
+      <c r="H14" s="10">
+        <v>0</v>
+      </c>
+      <c r="I14" s="10">
+        <v>0</v>
+      </c>
+      <c r="J14" s="10">
+        <v>0</v>
+      </c>
+      <c r="K14" s="10">
+        <v>0</v>
+      </c>
+      <c r="L14" s="10">
+        <v>0</v>
+      </c>
+      <c r="N14" s="11">
+        <v>0</v>
+      </c>
+      <c r="O14" s="8">
+        <v>0</v>
+      </c>
+      <c r="P14" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="12">
+        <v>120</v>
+      </c>
+      <c r="C15" s="12">
+        <v>150</v>
+      </c>
+      <c r="D15" s="12">
+        <v>180</v>
+      </c>
+      <c r="F15" s="10">
+        <v>120</v>
+      </c>
+      <c r="G15" s="10">
+        <v>80</v>
+      </c>
+      <c r="H15" s="10">
+        <v>80</v>
+      </c>
+      <c r="I15" s="10">
+        <v>140</v>
+      </c>
+      <c r="J15" s="10">
+        <v>160</v>
+      </c>
+      <c r="K15" s="10">
+        <v>160</v>
+      </c>
+      <c r="L15" s="10">
+        <v>200</v>
+      </c>
+      <c r="N15" s="11">
+        <v>90</v>
+      </c>
+      <c r="O15" s="8">
+        <v>100</v>
+      </c>
+      <c r="P15" s="8">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="12">
+        <v>120</v>
+      </c>
+      <c r="C16" s="12">
+        <v>150</v>
+      </c>
+      <c r="D16" s="12">
+        <v>180</v>
+      </c>
+      <c r="F16" s="10">
+        <v>80</v>
+      </c>
+      <c r="G16" s="10">
+        <v>80</v>
+      </c>
+      <c r="H16" s="10">
+        <v>80</v>
+      </c>
+      <c r="I16" s="10">
+        <v>80</v>
+      </c>
+      <c r="J16" s="10">
+        <v>80</v>
+      </c>
+      <c r="K16" s="10">
+        <v>80</v>
+      </c>
+      <c r="L16" s="10">
+        <v>100</v>
+      </c>
+      <c r="N16" s="11">
+        <v>80</v>
+      </c>
+      <c r="O16" s="8">
+        <v>80</v>
+      </c>
+      <c r="P16" s="8">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="12">
+        <v>120</v>
+      </c>
+      <c r="C17" s="12">
+        <v>150</v>
+      </c>
+      <c r="D17" s="12">
+        <v>180</v>
+      </c>
+      <c r="F17" s="10">
+        <v>80</v>
+      </c>
+      <c r="G17" s="10">
+        <v>150</v>
+      </c>
+      <c r="H17" s="10">
+        <v>180</v>
+      </c>
+      <c r="I17" s="10">
+        <v>80</v>
+      </c>
+      <c r="J17" s="10">
+        <v>80</v>
+      </c>
+      <c r="K17" s="10">
+        <v>80</v>
+      </c>
+      <c r="L17" s="10">
+        <v>100</v>
+      </c>
+      <c r="N17" s="11">
+        <v>80</v>
+      </c>
+      <c r="O17" s="8">
+        <v>80</v>
+      </c>
+      <c r="P17" s="8">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="12">
+        <v>100</v>
+      </c>
+      <c r="C18" s="12">
+        <v>100</v>
+      </c>
+      <c r="D18" s="12">
+        <v>100</v>
+      </c>
+      <c r="F18" s="10">
+        <v>80</v>
+      </c>
+      <c r="G18" s="10">
+        <v>80</v>
+      </c>
+      <c r="H18" s="10">
+        <v>80</v>
+      </c>
+      <c r="I18" s="10">
+        <v>80</v>
+      </c>
+      <c r="J18" s="10">
+        <v>80</v>
+      </c>
+      <c r="K18" s="10">
+        <v>80</v>
+      </c>
+      <c r="L18" s="10">
+        <v>100</v>
+      </c>
+      <c r="N18" s="11">
+        <v>120</v>
+      </c>
+      <c r="O18" s="8">
+        <v>150</v>
+      </c>
+      <c r="P18" s="8">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="12">
+        <v>100</v>
+      </c>
+      <c r="C19" s="12">
+        <v>100</v>
+      </c>
+      <c r="D19" s="12">
+        <v>100</v>
+      </c>
+      <c r="F19" s="10">
+        <v>80</v>
+      </c>
+      <c r="G19" s="10">
+        <v>80</v>
+      </c>
+      <c r="H19" s="10">
+        <v>80</v>
+      </c>
+      <c r="I19" s="10">
+        <v>80</v>
+      </c>
+      <c r="J19" s="10">
+        <v>80</v>
+      </c>
+      <c r="K19" s="10">
+        <v>80</v>
+      </c>
+      <c r="L19" s="10">
+        <v>100</v>
+      </c>
+      <c r="N19" s="11">
+        <v>80</v>
+      </c>
+      <c r="O19" s="8">
+        <v>80</v>
+      </c>
+      <c r="P19" s="8">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="12">
+        <v>100</v>
+      </c>
+      <c r="C20" s="12">
+        <v>100</v>
+      </c>
+      <c r="D20" s="12">
+        <v>100</v>
+      </c>
+      <c r="F20" s="10">
+        <v>80</v>
+      </c>
+      <c r="G20" s="10">
+        <v>80</v>
+      </c>
+      <c r="H20" s="10">
+        <v>80</v>
+      </c>
+      <c r="I20" s="10">
+        <v>80</v>
+      </c>
+      <c r="J20" s="10">
+        <v>80</v>
+      </c>
+      <c r="K20" s="10">
+        <v>80</v>
+      </c>
+      <c r="L20" s="10">
+        <v>100</v>
+      </c>
+      <c r="N20" s="11">
+        <v>80</v>
+      </c>
+      <c r="O20" s="8">
+        <v>80</v>
+      </c>
+      <c r="P20" s="8">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C48F968-6098-45C2-90F4-E48BCC11AF74}">
   <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O3" sqref="O3:O20"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L1" sqref="L1:N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3664,8 +5441,8 @@
   <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A19" sqref="A19"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1:J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4694,7 +6471,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" sqref="A1:A20"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5706,7 +7483,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I13" sqref="I13"/>
+      <selection pane="topRight" activeCell="I1" sqref="I1:I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6310,7 +8087,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" sqref="A1:A20"/>
+      <selection pane="topRight" activeCell="G1" sqref="G1:I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>